<commit_message>
Add new terms needed for PRISM project, details see: 20150506_NewTermRequest.xlsx
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@67777 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/doc/20150506_NewTermRequest.xlsx
+++ b/Load/src/ontology/doc/20150506_NewTermRequest.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>current term</t>
   </si>
@@ -90,9 +90,6 @@
     <t>A blood specimen that is located on a filter paper.</t>
   </si>
   <si>
-    <t>OBI or OBIB?</t>
-  </si>
-  <si>
     <t>peripheral blood mononuclear cell specimen (PBMC specimen)</t>
   </si>
   <si>
@@ -151,6 +148,18 @@
   </si>
   <si>
     <t>filter paper</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000129</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000128</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000127</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000126</t>
   </si>
 </sst>
 </file>
@@ -478,7 +487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -488,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,16 +523,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -531,19 +540,22 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
       <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -551,13 +563,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -566,10 +578,10 @@
         <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -577,7 +589,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -600,16 +612,16 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -617,22 +629,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
         <v>30</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -640,7 +652,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -661,7 +673,7 @@
     <hyperlink ref="D7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>